<commit_message>
addition of cyclic FIP comparison analysis
</commit_message>
<xml_diff>
--- a/fip_collab/2016_01_28_gsh_database_codes/interpolation_test.xlsx
+++ b/fip_collab/2016_01_28_gsh_database_codes/interpolation_test.xlsx
@@ -336,11 +336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="383164864"/>
-        <c:axId val="383164472"/>
+        <c:axId val="316014016"/>
+        <c:axId val="316007024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="383164864"/>
+        <c:axId val="316014016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -458,12 +458,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383164472"/>
+        <c:crossAx val="316007024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="383164472"/>
+        <c:axId val="316007024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0000000000000017E-5"/>
@@ -583,7 +583,577 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383164864"/>
+        <c:crossAx val="316014016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>euler basis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9999999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1E-8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0000000000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.9999999999999995E-21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>theta basis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9999999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1E-8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0000000000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.9999999999999995E-21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>en basis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9999999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1E-8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0000000000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.9999999999999995E-21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="370860624"/>
+        <c:axId val="317313400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="370860624"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+          <c:min val="1.0000000000000005E-9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="317313400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="317313400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370860624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -672,7 +1242,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1215,6 +2341,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1488,8 +2644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>